<commit_message>
data update - sept 17
</commit_message>
<xml_diff>
--- a/data/category_tree.xlsx
+++ b/data/category_tree.xlsx
@@ -4966,12 +4966,12 @@
   <dimension ref="A1:M1087"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.712962962963" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="20.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="23.712962962963" customWidth="1"/>
     <col min="3" max="3" width="12.712962962963" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>

</xml_diff>